<commit_message>
correct figures hw 2
</commit_message>
<xml_diff>
--- a/HW01_Notes/1D ss satd_Hull.xlsx
+++ b/HW01_Notes/1D ss satd_Hull.xlsx
@@ -10,13 +10,13 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="166" documentId="13_ncr:1_{0782B73B-6BEC-43BF-AA2A-643772B0639A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0D1DEA0D-D87A-4842-B17B-36A97E27F991}"/>
   <bookViews>
-    <workbookView xWindow="26320" yWindow="460" windowWidth="24580" windowHeight="26640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="460" windowWidth="24580" windowHeight="26640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="2" r:id="rId1"/>
     <sheet name="model and key plot" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -2704,7 +2704,7 @@
   <dimension ref="B3:T89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63"/>
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>